<commit_message>
Edited formatting of inducer final concentrations to allow for flowating points
</commit_message>
<xml_diff>
--- a/HTC_Scripting_Template_v3.xlsx
+++ b/HTC_Scripting_Template_v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eribertolopez/Documents/GitHub/Aquarium_HTC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA0B688-610D-5F49-BD3D-E13C6F51DBAA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B05B1A-B8C0-6749-9B15-9B60E4ACB96E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16760" xr2:uid="{72935FC3-A054-E347-8166-6079D9172055}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="27">
   <si>
     <t>Replicates</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Options</t>
   </si>
   <si>
-    <t>Antibiotics</t>
-  </si>
-  <si>
     <t>Control_Tag</t>
   </si>
   <si>
@@ -99,10 +96,16 @@
     <t>Yeast Glycerol Stock</t>
   </si>
   <si>
-    <t>0_nM, 5nM, 10nM, 25nM, 50nM, 75_nM, 100nM</t>
-  </si>
-  <si>
     <t>0_nM, 50nM, 75_nM, 100_nM</t>
+  </si>
+  <si>
+    <t>Antibiotic_name</t>
+  </si>
+  <si>
+    <t>Antibiotic_FinalConcentration</t>
+  </si>
+  <si>
+    <t>0_nM, 0.55nM, 0.10nM, 25nM, 50nM, 75_nM, 100nM</t>
   </si>
 </sst>
 </file>
@@ -457,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA43CC9C-4A5E-C845-A810-8D25623061CE}">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -479,9 +482,11 @@
     <col min="12" max="12" width="27.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22.33203125" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -492,13 +497,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -525,13 +530,16 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="P1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -545,10 +553,10 @@
         <v>6390</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -562,16 +570,16 @@
         <v>6390</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3" t="s">
         <v>7</v>
       </c>
       <c r="J3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -585,22 +593,22 @@
         <v>6390</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I4" t="s">
         <v>7</v>
       </c>
       <c r="J4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K4" t="s">
         <v>9</v>
       </c>
       <c r="L4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -611,19 +619,19 @@
         <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5" t="s">
         <v>7</v>
       </c>
       <c r="J5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -634,19 +642,19 @@
         <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I6" t="s">
         <v>7</v>
       </c>
       <c r="J6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -657,25 +665,25 @@
         <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I7" t="s">
         <v>7</v>
       </c>
       <c r="J7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K7" t="s">
         <v>9</v>
       </c>
       <c r="L7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -686,25 +694,25 @@
         <v>14</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I8" t="s">
         <v>7</v>
       </c>
       <c r="J8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K8" t="s">
         <v>9</v>
       </c>
       <c r="L8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -715,19 +723,19 @@
         <v>14</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K9" t="s">
         <v>9</v>
       </c>
       <c r="L9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -744,10 +752,10 @@
         <v>6390</v>
       </c>
       <c r="G10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -761,13 +769,13 @@
         <v>15</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -778,13 +786,13 @@
         <v>14</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -798,7 +806,7 @@
         <v>6390</v>
       </c>
       <c r="G13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edits to python scripts and excel template
</commit_message>
<xml_diff>
--- a/HTC_Scripting_Template_v3.xlsx
+++ b/HTC_Scripting_Template_v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eribertolopez/Documents/GitHub/Aquarium_HTC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C86B962-F82E-3441-B206-72648AA4FA46}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04279E6-B16A-9049-BF36-D19346B7D3A9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16760" xr2:uid="{72935FC3-A054-E347-8166-6079D9172055}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="32">
   <si>
     <t>Replicates</t>
   </si>
@@ -108,13 +108,19 @@
     <t>0_nM, 0.55nM, 0.10nM, 25nM, 50nM, 75_nM, 100nM</t>
   </si>
   <si>
-    <t>{"reagents": {"Ethanol": {"qty": 70, "units": "percent"} }, "temperature": {"qty": 37, "units": C}, "duration": {"qty": 15, "units": "minute"}</t>
-  </si>
-  <si>
     <t>Ampicillin Antibiotic</t>
   </si>
   <si>
     <t>0.1_ug/mL</t>
+  </si>
+  <si>
+    <t>200_ug/mL</t>
+  </si>
+  <si>
+    <t>0.1ug/mL</t>
+  </si>
+  <si>
+    <t>{"reagents": {"Ethanol": {"qty": 70, "units": "percent"} }, "temperature": {"qty": 37, "units": "C"}, "duration": {"qty": 15, "units": "minute"}}</t>
   </si>
 </sst>
 </file>
@@ -471,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA43CC9C-4A5E-C845-A810-8D25623061CE}">
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -566,13 +572,13 @@
         <v>22</v>
       </c>
       <c r="O2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" t="s">
         <v>28</v>
       </c>
-      <c r="P2" t="s">
-        <v>29</v>
-      </c>
       <c r="Q2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -701,6 +707,12 @@
       <c r="L7" t="s">
         <v>23</v>
       </c>
+      <c r="O7" t="s">
+        <v>27</v>
+      </c>
+      <c r="P7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -752,6 +764,15 @@
       </c>
       <c r="L9" t="s">
         <v>23</v>
+      </c>
+      <c r="O9" t="s">
+        <v>27</v>
+      </c>
+      <c r="P9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>